<commit_message>
Extend age tables for lookup completeness
</commit_message>
<xml_diff>
--- a/InputData/hydgn/HESD/Hydrogen Equipment Survival Data.xlsx
+++ b/InputData/hydgn/HESD/Hydrogen Equipment Survival Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\hydgn\HPESC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\hydgn\HESD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE7D3FF-1516-477E-9644-88FA2BA57835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF48578-9A6B-47D2-9D9A-254E77A2A153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59085" yWindow="1740" windowWidth="24900" windowHeight="14490" xr2:uid="{D7D4D39B-1881-45DC-8052-5A256985CC24}"/>
+    <workbookView xWindow="34185" yWindow="1470" windowWidth="21600" windowHeight="11175" activeTab="3" xr2:uid="{D7D4D39B-1881-45DC-8052-5A256985CC24}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -12506,24 +12506,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA4E951-0C61-4C70-BCC5-3459910506B3}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="65.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -12531,57 +12531,57 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>2008</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20</v>
       </c>
@@ -12598,23 +12598,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460F6A24-E425-4092-8D01-D6B9CD51ADEB}">
   <dimension ref="A2:BU89"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N102" sqref="N102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="73" width="6.54296875" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="73" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -12649,7 +12649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -12687,7 +12687,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -12725,7 +12725,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -12763,7 +12763,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>21</v>
       </c>
@@ -12801,7 +12801,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>22</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>23</v>
       </c>
@@ -12877,7 +12877,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>24</v>
       </c>
@@ -12915,7 +12915,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>25</v>
       </c>
@@ -12953,7 +12953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>26</v>
       </c>
@@ -12991,7 +12991,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>27</v>
       </c>
@@ -13029,7 +13029,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>28</v>
       </c>
@@ -13067,7 +13067,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>29</v>
       </c>
@@ -13105,7 +13105,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -13143,7 +13143,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>31</v>
       </c>
@@ -13181,7 +13181,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -13219,7 +13219,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>43</v>
       </c>
@@ -13230,17 +13230,17 @@
         <v>4.0409228976360727E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:73" ht="22" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:73" ht="22.5" x14ac:dyDescent="0.4">
       <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>0</v>
       </c>
@@ -13455,7 +13455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>27</v>
       </c>
@@ -13744,7 +13744,7 @@
         <v>0.96864675610454498</v>
       </c>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>29</v>
       </c>
@@ -14033,7 +14033,7 @@
         <v>0.9960808578779623</v>
       </c>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -14322,7 +14322,7 @@
         <v>0.98604189770297412</v>
       </c>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>41</v>
       </c>
@@ -14611,7 +14611,7 @@
         <v>0.98744309417195952</v>
       </c>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -14900,7 +14900,7 @@
         <v>0.99999999901056857</v>
       </c>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -15189,7 +15189,7 @@
         <v>0.8877834661564773</v>
       </c>
     </row>
-    <row r="33" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -15478,7 +15478,7 @@
         <v>0.99260488246384015</v>
       </c>
     </row>
-    <row r="34" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -15767,7 +15767,7 @@
         <v>0.94049868236716638</v>
       </c>
     </row>
-    <row r="35" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -16056,7 +16056,7 @@
         <v>0.9964176201456928</v>
       </c>
     </row>
-    <row r="36" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -16345,7 +16345,7 @@
         <v>0.98749909623218113</v>
       </c>
     </row>
-    <row r="37" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -16634,7 +16634,7 @@
         <v>0.94809341565716188</v>
       </c>
     </row>
-    <row r="38" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -16923,7 +16923,7 @@
         <v>0.97745349576445428</v>
       </c>
     </row>
-    <row r="39" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -17212,7 +17212,7 @@
         <v>0.99861736150173053</v>
       </c>
     </row>
-    <row r="40" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -17501,7 +17501,7 @@
         <v>0.81815164815773878</v>
       </c>
     </row>
-    <row r="41" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -17790,7 +17790,7 @@
         <v>0.97665058093177115</v>
       </c>
     </row>
-    <row r="42" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
@@ -18079,42 +18079,42 @@
         <v>0.99748734272093731</v>
       </c>
     </row>
-    <row r="43" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:73" x14ac:dyDescent="0.25">
       <c r="W43" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="2:73" ht="22" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:73" ht="22.5" x14ac:dyDescent="0.4">
       <c r="B45" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:73" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:73" ht="18" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="20.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:4" ht="21.75" x14ac:dyDescent="0.4">
       <c r="B49" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>9</v>
       </c>
@@ -18122,7 +18122,7 @@
         <v>27.9</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>10</v>
       </c>
@@ -18130,7 +18130,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>11</v>
       </c>
@@ -18138,7 +18138,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>21</v>
       </c>
@@ -18146,7 +18146,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>22</v>
       </c>
@@ -18154,7 +18154,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>23</v>
       </c>
@@ -18165,7 +18165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>24</v>
       </c>
@@ -18173,7 +18173,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>25</v>
       </c>
@@ -18181,7 +18181,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>26</v>
       </c>
@@ -18189,7 +18189,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>27</v>
       </c>
@@ -18197,7 +18197,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>28</v>
       </c>
@@ -18205,7 +18205,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>29</v>
       </c>
@@ -18213,7 +18213,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>12</v>
       </c>
@@ -18221,7 +18221,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="66" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>31</v>
       </c>
@@ -18229,7 +18229,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>13</v>
       </c>
@@ -18237,7 +18237,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="68" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>23</v>
       </c>
@@ -18249,12 +18249,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:73" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>0</v>
       </c>
@@ -18469,7 +18469,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>27</v>
       </c>
@@ -18758,7 +18758,7 @@
         <v>3.1353243895455019E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>29</v>
       </c>
@@ -19047,7 +19047,7 @@
         <v>3.9191421220376998E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>42</v>
       </c>
@@ -19336,7 +19336,7 @@
         <v>1.3958102297025876E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>41</v>
       </c>
@@ -19625,7 +19625,7 @@
         <v>1.2556905828040477E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>30</v>
       </c>
@@ -19914,7 +19914,7 @@
         <v>9.8943142567975428E-10</v>
       </c>
     </row>
-    <row r="77" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>31</v>
       </c>
@@ -20203,7 +20203,7 @@
         <v>0.1122165338435227</v>
       </c>
     </row>
-    <row r="78" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>32</v>
       </c>
@@ -20492,7 +20492,7 @@
         <v>7.3951175361598454E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>33</v>
       </c>
@@ -20781,7 +20781,7 @@
         <v>5.9501317632833617E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>34</v>
       </c>
@@ -21070,7 +21070,7 @@
         <v>3.582379854307205E-3</v>
       </c>
     </row>
-    <row r="81" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>35</v>
       </c>
@@ -21359,7 +21359,7 @@
         <v>1.2500903767818872E-2</v>
       </c>
     </row>
-    <row r="82" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>36</v>
       </c>
@@ -21648,7 +21648,7 @@
         <v>5.1906584342838125E-2</v>
       </c>
     </row>
-    <row r="83" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>37</v>
       </c>
@@ -21937,7 +21937,7 @@
         <v>2.2546504235545717E-2</v>
       </c>
     </row>
-    <row r="84" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>38</v>
       </c>
@@ -22226,7 +22226,7 @@
         <v>1.3826384982694728E-3</v>
       </c>
     </row>
-    <row r="85" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>39</v>
       </c>
@@ -22515,7 +22515,7 @@
         <v>0.18184835184226122</v>
       </c>
     </row>
-    <row r="86" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>40</v>
       </c>
@@ -22804,7 +22804,7 @@
         <v>2.3349419068228849E-2</v>
       </c>
     </row>
-    <row r="87" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>43</v>
       </c>
@@ -23092,7 +23092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B88" s="12" t="s">
         <v>59</v>
       </c>
@@ -23381,7 +23381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:73" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B89" s="12" t="s">
         <v>60</v>
       </c>
@@ -23686,13 +23686,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="211" width="10.453125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="211" width="10.42578125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:211" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -24327,7 +24327,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:211" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:211" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -25032,7 +25032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:211" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:211" x14ac:dyDescent="0.25">
       <c r="DV6"/>
     </row>
   </sheetData>
@@ -25045,18 +25045,18 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:BT2"/>
+  <dimension ref="A1:HD2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BS17" sqref="BS17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -25270,8 +25270,428 @@
       <c r="BT1">
         <v>70</v>
       </c>
+      <c r="BU1">
+        <v>71</v>
+      </c>
+      <c r="BV1">
+        <v>72</v>
+      </c>
+      <c r="BW1">
+        <v>73</v>
+      </c>
+      <c r="BX1">
+        <v>74</v>
+      </c>
+      <c r="BY1">
+        <v>75</v>
+      </c>
+      <c r="BZ1">
+        <v>76</v>
+      </c>
+      <c r="CA1">
+        <v>77</v>
+      </c>
+      <c r="CB1">
+        <v>78</v>
+      </c>
+      <c r="CC1">
+        <v>79</v>
+      </c>
+      <c r="CD1">
+        <v>80</v>
+      </c>
+      <c r="CE1">
+        <v>81</v>
+      </c>
+      <c r="CF1">
+        <v>82</v>
+      </c>
+      <c r="CG1">
+        <v>83</v>
+      </c>
+      <c r="CH1">
+        <v>84</v>
+      </c>
+      <c r="CI1">
+        <v>85</v>
+      </c>
+      <c r="CJ1">
+        <v>86</v>
+      </c>
+      <c r="CK1">
+        <v>87</v>
+      </c>
+      <c r="CL1">
+        <v>88</v>
+      </c>
+      <c r="CM1">
+        <v>89</v>
+      </c>
+      <c r="CN1">
+        <v>90</v>
+      </c>
+      <c r="CO1">
+        <v>91</v>
+      </c>
+      <c r="CP1">
+        <v>92</v>
+      </c>
+      <c r="CQ1">
+        <v>93</v>
+      </c>
+      <c r="CR1">
+        <v>94</v>
+      </c>
+      <c r="CS1">
+        <v>95</v>
+      </c>
+      <c r="CT1">
+        <v>96</v>
+      </c>
+      <c r="CU1">
+        <v>97</v>
+      </c>
+      <c r="CV1">
+        <v>98</v>
+      </c>
+      <c r="CW1">
+        <v>99</v>
+      </c>
+      <c r="CX1">
+        <v>100</v>
+      </c>
+      <c r="CY1">
+        <v>101</v>
+      </c>
+      <c r="CZ1">
+        <v>102</v>
+      </c>
+      <c r="DA1">
+        <v>103</v>
+      </c>
+      <c r="DB1">
+        <v>104</v>
+      </c>
+      <c r="DC1">
+        <v>105</v>
+      </c>
+      <c r="DD1">
+        <v>106</v>
+      </c>
+      <c r="DE1">
+        <v>107</v>
+      </c>
+      <c r="DF1">
+        <v>108</v>
+      </c>
+      <c r="DG1">
+        <v>109</v>
+      </c>
+      <c r="DH1">
+        <v>110</v>
+      </c>
+      <c r="DI1">
+        <v>111</v>
+      </c>
+      <c r="DJ1">
+        <v>112</v>
+      </c>
+      <c r="DK1">
+        <v>113</v>
+      </c>
+      <c r="DL1">
+        <v>114</v>
+      </c>
+      <c r="DM1">
+        <v>115</v>
+      </c>
+      <c r="DN1">
+        <v>116</v>
+      </c>
+      <c r="DO1">
+        <v>117</v>
+      </c>
+      <c r="DP1">
+        <v>118</v>
+      </c>
+      <c r="DQ1">
+        <v>119</v>
+      </c>
+      <c r="DR1">
+        <v>120</v>
+      </c>
+      <c r="DS1">
+        <v>121</v>
+      </c>
+      <c r="DT1">
+        <v>122</v>
+      </c>
+      <c r="DU1">
+        <v>123</v>
+      </c>
+      <c r="DV1">
+        <v>124</v>
+      </c>
+      <c r="DW1">
+        <v>125</v>
+      </c>
+      <c r="DX1">
+        <v>126</v>
+      </c>
+      <c r="DY1">
+        <v>127</v>
+      </c>
+      <c r="DZ1">
+        <v>128</v>
+      </c>
+      <c r="EA1">
+        <v>129</v>
+      </c>
+      <c r="EB1">
+        <v>130</v>
+      </c>
+      <c r="EC1">
+        <v>131</v>
+      </c>
+      <c r="ED1">
+        <v>132</v>
+      </c>
+      <c r="EE1">
+        <v>133</v>
+      </c>
+      <c r="EF1">
+        <v>134</v>
+      </c>
+      <c r="EG1">
+        <v>135</v>
+      </c>
+      <c r="EH1">
+        <v>136</v>
+      </c>
+      <c r="EI1">
+        <v>137</v>
+      </c>
+      <c r="EJ1">
+        <v>138</v>
+      </c>
+      <c r="EK1">
+        <v>139</v>
+      </c>
+      <c r="EL1">
+        <v>140</v>
+      </c>
+      <c r="EM1">
+        <v>141</v>
+      </c>
+      <c r="EN1">
+        <v>142</v>
+      </c>
+      <c r="EO1">
+        <v>143</v>
+      </c>
+      <c r="EP1">
+        <v>144</v>
+      </c>
+      <c r="EQ1">
+        <v>145</v>
+      </c>
+      <c r="ER1">
+        <v>146</v>
+      </c>
+      <c r="ES1">
+        <v>147</v>
+      </c>
+      <c r="ET1">
+        <v>148</v>
+      </c>
+      <c r="EU1">
+        <v>149</v>
+      </c>
+      <c r="EV1">
+        <v>150</v>
+      </c>
+      <c r="EW1">
+        <v>151</v>
+      </c>
+      <c r="EX1">
+        <v>152</v>
+      </c>
+      <c r="EY1">
+        <v>153</v>
+      </c>
+      <c r="EZ1">
+        <v>154</v>
+      </c>
+      <c r="FA1">
+        <v>155</v>
+      </c>
+      <c r="FB1">
+        <v>156</v>
+      </c>
+      <c r="FC1">
+        <v>157</v>
+      </c>
+      <c r="FD1">
+        <v>158</v>
+      </c>
+      <c r="FE1">
+        <v>159</v>
+      </c>
+      <c r="FF1">
+        <v>160</v>
+      </c>
+      <c r="FG1">
+        <v>161</v>
+      </c>
+      <c r="FH1">
+        <v>162</v>
+      </c>
+      <c r="FI1">
+        <v>163</v>
+      </c>
+      <c r="FJ1">
+        <v>164</v>
+      </c>
+      <c r="FK1">
+        <v>165</v>
+      </c>
+      <c r="FL1">
+        <v>166</v>
+      </c>
+      <c r="FM1">
+        <v>167</v>
+      </c>
+      <c r="FN1">
+        <v>168</v>
+      </c>
+      <c r="FO1">
+        <v>169</v>
+      </c>
+      <c r="FP1">
+        <v>170</v>
+      </c>
+      <c r="FQ1">
+        <v>171</v>
+      </c>
+      <c r="FR1">
+        <v>172</v>
+      </c>
+      <c r="FS1">
+        <v>173</v>
+      </c>
+      <c r="FT1">
+        <v>174</v>
+      </c>
+      <c r="FU1">
+        <v>175</v>
+      </c>
+      <c r="FV1">
+        <v>176</v>
+      </c>
+      <c r="FW1">
+        <v>177</v>
+      </c>
+      <c r="FX1">
+        <v>178</v>
+      </c>
+      <c r="FY1">
+        <v>179</v>
+      </c>
+      <c r="FZ1">
+        <v>180</v>
+      </c>
+      <c r="GA1">
+        <v>181</v>
+      </c>
+      <c r="GB1">
+        <v>182</v>
+      </c>
+      <c r="GC1">
+        <v>183</v>
+      </c>
+      <c r="GD1">
+        <v>184</v>
+      </c>
+      <c r="GE1">
+        <v>185</v>
+      </c>
+      <c r="GF1">
+        <v>186</v>
+      </c>
+      <c r="GG1">
+        <v>187</v>
+      </c>
+      <c r="GH1">
+        <v>188</v>
+      </c>
+      <c r="GI1">
+        <v>189</v>
+      </c>
+      <c r="GJ1">
+        <v>190</v>
+      </c>
+      <c r="GK1">
+        <v>191</v>
+      </c>
+      <c r="GL1">
+        <v>192</v>
+      </c>
+      <c r="GM1">
+        <v>193</v>
+      </c>
+      <c r="GN1">
+        <v>194</v>
+      </c>
+      <c r="GO1">
+        <v>195</v>
+      </c>
+      <c r="GP1">
+        <v>196</v>
+      </c>
+      <c r="GQ1">
+        <v>197</v>
+      </c>
+      <c r="GR1">
+        <v>198</v>
+      </c>
+      <c r="GS1">
+        <v>199</v>
+      </c>
+      <c r="GT1">
+        <v>200</v>
+      </c>
+      <c r="GU1">
+        <v>201</v>
+      </c>
+      <c r="GV1">
+        <v>202</v>
+      </c>
+      <c r="GW1">
+        <v>203</v>
+      </c>
+      <c r="GX1">
+        <v>204</v>
+      </c>
+      <c r="GY1">
+        <v>205</v>
+      </c>
+      <c r="GZ1">
+        <v>206</v>
+      </c>
+      <c r="HA1">
+        <v>207</v>
+      </c>
+      <c r="HB1">
+        <v>208</v>
+      </c>
+      <c r="HC1">
+        <v>209</v>
+      </c>
+      <c r="HD1">
+        <v>210</v>
+      </c>
     </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:212" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -25557,6 +25977,426 @@
       </c>
       <c r="BT2">
         <f>Calcs!BU89</f>
+        <v>1</v>
+      </c>
+      <c r="BU2">
+        <v>1</v>
+      </c>
+      <c r="BV2">
+        <v>1</v>
+      </c>
+      <c r="BW2">
+        <v>1</v>
+      </c>
+      <c r="BX2">
+        <v>1</v>
+      </c>
+      <c r="BY2">
+        <v>1</v>
+      </c>
+      <c r="BZ2">
+        <v>1</v>
+      </c>
+      <c r="CA2">
+        <v>1</v>
+      </c>
+      <c r="CB2">
+        <v>1</v>
+      </c>
+      <c r="CC2">
+        <v>1</v>
+      </c>
+      <c r="CD2">
+        <v>1</v>
+      </c>
+      <c r="CE2">
+        <v>1</v>
+      </c>
+      <c r="CF2">
+        <v>1</v>
+      </c>
+      <c r="CG2">
+        <v>1</v>
+      </c>
+      <c r="CH2">
+        <v>1</v>
+      </c>
+      <c r="CI2">
+        <v>1</v>
+      </c>
+      <c r="CJ2">
+        <v>1</v>
+      </c>
+      <c r="CK2">
+        <v>1</v>
+      </c>
+      <c r="CL2">
+        <v>1</v>
+      </c>
+      <c r="CM2">
+        <v>1</v>
+      </c>
+      <c r="CN2">
+        <v>1</v>
+      </c>
+      <c r="CO2">
+        <v>1</v>
+      </c>
+      <c r="CP2">
+        <v>1</v>
+      </c>
+      <c r="CQ2">
+        <v>1</v>
+      </c>
+      <c r="CR2">
+        <v>1</v>
+      </c>
+      <c r="CS2">
+        <v>1</v>
+      </c>
+      <c r="CT2">
+        <v>1</v>
+      </c>
+      <c r="CU2">
+        <v>1</v>
+      </c>
+      <c r="CV2">
+        <v>1</v>
+      </c>
+      <c r="CW2">
+        <v>1</v>
+      </c>
+      <c r="CX2">
+        <v>1</v>
+      </c>
+      <c r="CY2">
+        <v>1</v>
+      </c>
+      <c r="CZ2">
+        <v>1</v>
+      </c>
+      <c r="DA2">
+        <v>1</v>
+      </c>
+      <c r="DB2">
+        <v>1</v>
+      </c>
+      <c r="DC2">
+        <v>1</v>
+      </c>
+      <c r="DD2">
+        <v>1</v>
+      </c>
+      <c r="DE2">
+        <v>1</v>
+      </c>
+      <c r="DF2">
+        <v>1</v>
+      </c>
+      <c r="DG2">
+        <v>1</v>
+      </c>
+      <c r="DH2">
+        <v>1</v>
+      </c>
+      <c r="DI2">
+        <v>1</v>
+      </c>
+      <c r="DJ2">
+        <v>1</v>
+      </c>
+      <c r="DK2">
+        <v>1</v>
+      </c>
+      <c r="DL2">
+        <v>1</v>
+      </c>
+      <c r="DM2">
+        <v>1</v>
+      </c>
+      <c r="DN2">
+        <v>1</v>
+      </c>
+      <c r="DO2">
+        <v>1</v>
+      </c>
+      <c r="DP2">
+        <v>1</v>
+      </c>
+      <c r="DQ2">
+        <v>1</v>
+      </c>
+      <c r="DR2">
+        <v>1</v>
+      </c>
+      <c r="DS2">
+        <v>1</v>
+      </c>
+      <c r="DT2">
+        <v>1</v>
+      </c>
+      <c r="DU2">
+        <v>1</v>
+      </c>
+      <c r="DV2">
+        <v>1</v>
+      </c>
+      <c r="DW2">
+        <v>1</v>
+      </c>
+      <c r="DX2">
+        <v>1</v>
+      </c>
+      <c r="DY2">
+        <v>1</v>
+      </c>
+      <c r="DZ2">
+        <v>1</v>
+      </c>
+      <c r="EA2">
+        <v>1</v>
+      </c>
+      <c r="EB2">
+        <v>1</v>
+      </c>
+      <c r="EC2">
+        <v>1</v>
+      </c>
+      <c r="ED2">
+        <v>1</v>
+      </c>
+      <c r="EE2">
+        <v>1</v>
+      </c>
+      <c r="EF2">
+        <v>1</v>
+      </c>
+      <c r="EG2">
+        <v>1</v>
+      </c>
+      <c r="EH2">
+        <v>1</v>
+      </c>
+      <c r="EI2">
+        <v>1</v>
+      </c>
+      <c r="EJ2">
+        <v>1</v>
+      </c>
+      <c r="EK2">
+        <v>1</v>
+      </c>
+      <c r="EL2">
+        <v>1</v>
+      </c>
+      <c r="EM2">
+        <v>1</v>
+      </c>
+      <c r="EN2">
+        <v>1</v>
+      </c>
+      <c r="EO2">
+        <v>1</v>
+      </c>
+      <c r="EP2">
+        <v>1</v>
+      </c>
+      <c r="EQ2">
+        <v>1</v>
+      </c>
+      <c r="ER2">
+        <v>1</v>
+      </c>
+      <c r="ES2">
+        <v>1</v>
+      </c>
+      <c r="ET2">
+        <v>1</v>
+      </c>
+      <c r="EU2">
+        <v>1</v>
+      </c>
+      <c r="EV2">
+        <v>1</v>
+      </c>
+      <c r="EW2">
+        <v>1</v>
+      </c>
+      <c r="EX2">
+        <v>1</v>
+      </c>
+      <c r="EY2">
+        <v>1</v>
+      </c>
+      <c r="EZ2">
+        <v>1</v>
+      </c>
+      <c r="FA2">
+        <v>1</v>
+      </c>
+      <c r="FB2">
+        <v>1</v>
+      </c>
+      <c r="FC2">
+        <v>1</v>
+      </c>
+      <c r="FD2">
+        <v>1</v>
+      </c>
+      <c r="FE2">
+        <v>1</v>
+      </c>
+      <c r="FF2">
+        <v>1</v>
+      </c>
+      <c r="FG2">
+        <v>1</v>
+      </c>
+      <c r="FH2">
+        <v>1</v>
+      </c>
+      <c r="FI2">
+        <v>1</v>
+      </c>
+      <c r="FJ2">
+        <v>1</v>
+      </c>
+      <c r="FK2">
+        <v>1</v>
+      </c>
+      <c r="FL2">
+        <v>1</v>
+      </c>
+      <c r="FM2">
+        <v>1</v>
+      </c>
+      <c r="FN2">
+        <v>1</v>
+      </c>
+      <c r="FO2">
+        <v>1</v>
+      </c>
+      <c r="FP2">
+        <v>1</v>
+      </c>
+      <c r="FQ2">
+        <v>1</v>
+      </c>
+      <c r="FR2">
+        <v>1</v>
+      </c>
+      <c r="FS2">
+        <v>1</v>
+      </c>
+      <c r="FT2">
+        <v>1</v>
+      </c>
+      <c r="FU2">
+        <v>1</v>
+      </c>
+      <c r="FV2">
+        <v>1</v>
+      </c>
+      <c r="FW2">
+        <v>1</v>
+      </c>
+      <c r="FX2">
+        <v>1</v>
+      </c>
+      <c r="FY2">
+        <v>1</v>
+      </c>
+      <c r="FZ2">
+        <v>1</v>
+      </c>
+      <c r="GA2">
+        <v>1</v>
+      </c>
+      <c r="GB2">
+        <v>1</v>
+      </c>
+      <c r="GC2">
+        <v>1</v>
+      </c>
+      <c r="GD2">
+        <v>1</v>
+      </c>
+      <c r="GE2">
+        <v>1</v>
+      </c>
+      <c r="GF2">
+        <v>1</v>
+      </c>
+      <c r="GG2">
+        <v>1</v>
+      </c>
+      <c r="GH2">
+        <v>1</v>
+      </c>
+      <c r="GI2">
+        <v>1</v>
+      </c>
+      <c r="GJ2">
+        <v>1</v>
+      </c>
+      <c r="GK2">
+        <v>1</v>
+      </c>
+      <c r="GL2">
+        <v>1</v>
+      </c>
+      <c r="GM2">
+        <v>1</v>
+      </c>
+      <c r="GN2">
+        <v>1</v>
+      </c>
+      <c r="GO2">
+        <v>1</v>
+      </c>
+      <c r="GP2">
+        <v>1</v>
+      </c>
+      <c r="GQ2">
+        <v>1</v>
+      </c>
+      <c r="GR2">
+        <v>1</v>
+      </c>
+      <c r="GS2">
+        <v>1</v>
+      </c>
+      <c r="GT2">
+        <v>1</v>
+      </c>
+      <c r="GU2">
+        <v>1</v>
+      </c>
+      <c r="GV2">
+        <v>1</v>
+      </c>
+      <c r="GW2">
+        <v>1</v>
+      </c>
+      <c r="GX2">
+        <v>1</v>
+      </c>
+      <c r="GY2">
+        <v>1</v>
+      </c>
+      <c r="GZ2">
+        <v>1</v>
+      </c>
+      <c r="HA2">
+        <v>1</v>
+      </c>
+      <c r="HB2">
+        <v>1</v>
+      </c>
+      <c r="HC2">
+        <v>1</v>
+      </c>
+      <c r="HD2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Shortens vintage subscript to start at 1950
</commit_message>
<xml_diff>
--- a/InputData/hydgn/HESD/Hydrogen Equipment Survival Data.xlsx
+++ b/InputData/hydgn/HESD/Hydrogen Equipment Survival Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\hydgn\HESD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF48578-9A6B-47D2-9D9A-254E77A2A153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B32DA8-C80F-4210-9EF0-EC237A3A2C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34185" yWindow="1470" windowWidth="21600" windowHeight="11175" activeTab="3" xr2:uid="{D7D4D39B-1881-45DC-8052-5A256985CC24}"/>
+    <workbookView xWindow="31590" yWindow="1515" windowWidth="24255" windowHeight="15525" activeTab="2" xr2:uid="{D7D4D39B-1881-45DC-8052-5A256985CC24}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="216">
   <si>
     <t>TABLE 4 ESTIMATED REGRESSION COEFFICIENTS: MACHINERY (3 YEARS DISCARD)</t>
   </si>
@@ -511,183 +511,6 @@
   </si>
   <si>
     <t>dimensionless (% of exisitng industrial equipment)</t>
-  </si>
-  <si>
-    <t>Vintage1891</t>
-  </si>
-  <si>
-    <t>Vintage1892</t>
-  </si>
-  <si>
-    <t>Vintage1893</t>
-  </si>
-  <si>
-    <t>Vintage1894</t>
-  </si>
-  <si>
-    <t>Vintage1895</t>
-  </si>
-  <si>
-    <t>Vintage1896</t>
-  </si>
-  <si>
-    <t>Vintage1897</t>
-  </si>
-  <si>
-    <t>Vintage1898</t>
-  </si>
-  <si>
-    <t>Vintage1899</t>
-  </si>
-  <si>
-    <t>Vintage1900</t>
-  </si>
-  <si>
-    <t>Vintage1901</t>
-  </si>
-  <si>
-    <t>Vintage1902</t>
-  </si>
-  <si>
-    <t>Vintage1903</t>
-  </si>
-  <si>
-    <t>Vintage1904</t>
-  </si>
-  <si>
-    <t>Vintage1905</t>
-  </si>
-  <si>
-    <t>Vintage1906</t>
-  </si>
-  <si>
-    <t>Vintage1907</t>
-  </si>
-  <si>
-    <t>Vintage1908</t>
-  </si>
-  <si>
-    <t>Vintage1909</t>
-  </si>
-  <si>
-    <t>Vintage1910</t>
-  </si>
-  <si>
-    <t>Vintage1911</t>
-  </si>
-  <si>
-    <t>Vintage1912</t>
-  </si>
-  <si>
-    <t>Vintage1913</t>
-  </si>
-  <si>
-    <t>Vintage1914</t>
-  </si>
-  <si>
-    <t>Vintage1915</t>
-  </si>
-  <si>
-    <t>Vintage1916</t>
-  </si>
-  <si>
-    <t>Vintage1917</t>
-  </si>
-  <si>
-    <t>Vintage1918</t>
-  </si>
-  <si>
-    <t>Vintage1919</t>
-  </si>
-  <si>
-    <t>Vintage1920</t>
-  </si>
-  <si>
-    <t>Vintage1921</t>
-  </si>
-  <si>
-    <t>Vintage1922</t>
-  </si>
-  <si>
-    <t>Vintage1923</t>
-  </si>
-  <si>
-    <t>Vintage1924</t>
-  </si>
-  <si>
-    <t>Vintage1925</t>
-  </si>
-  <si>
-    <t>Vintage1926</t>
-  </si>
-  <si>
-    <t>Vintage1927</t>
-  </si>
-  <si>
-    <t>Vintage1928</t>
-  </si>
-  <si>
-    <t>Vintage1929</t>
-  </si>
-  <si>
-    <t>Vintage1930</t>
-  </si>
-  <si>
-    <t>Vintage1931</t>
-  </si>
-  <si>
-    <t>Vintage1932</t>
-  </si>
-  <si>
-    <t>Vintage1933</t>
-  </si>
-  <si>
-    <t>Vintage1934</t>
-  </si>
-  <si>
-    <t>Vintage1935</t>
-  </si>
-  <si>
-    <t>Vintage1936</t>
-  </si>
-  <si>
-    <t>Vintage1937</t>
-  </si>
-  <si>
-    <t>Vintage1938</t>
-  </si>
-  <si>
-    <t>Vintage1939</t>
-  </si>
-  <si>
-    <t>Vintage1940</t>
-  </si>
-  <si>
-    <t>Vintage1941</t>
-  </si>
-  <si>
-    <t>Vintage1942</t>
-  </si>
-  <si>
-    <t>Vintage1943</t>
-  </si>
-  <si>
-    <t>Vintage1944</t>
-  </si>
-  <si>
-    <t>Vintage1945</t>
-  </si>
-  <si>
-    <t>Vintage1946</t>
-  </si>
-  <si>
-    <t>Vintage1947</t>
-  </si>
-  <si>
-    <t>Vintage1948</t>
-  </si>
-  <si>
-    <t>Vintage1949</t>
   </si>
   <si>
     <t>Vintage1950</t>
@@ -12508,22 +12331,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -12531,57 +12354,57 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7">
         <v>2008</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>20</v>
       </c>
@@ -12602,19 +12425,19 @@
       <selection activeCell="N102" sqref="N102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="73" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="73" width="6.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -12649,7 +12472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -12687,7 +12510,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -12725,7 +12548,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -12763,7 +12586,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>21</v>
       </c>
@@ -12801,7 +12624,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>22</v>
       </c>
@@ -12839,7 +12662,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>23</v>
       </c>
@@ -12877,7 +12700,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>24</v>
       </c>
@@ -12915,7 +12738,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>25</v>
       </c>
@@ -12953,7 +12776,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>26</v>
       </c>
@@ -12991,7 +12814,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>27</v>
       </c>
@@ -13029,7 +12852,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>28</v>
       </c>
@@ -13067,7 +12890,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>29</v>
       </c>
@@ -13105,7 +12928,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -13143,7 +12966,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>31</v>
       </c>
@@ -13181,7 +13004,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -13219,7 +13042,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>43</v>
       </c>
@@ -13230,17 +13053,17 @@
         <v>4.0409228976360727E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:73" ht="22.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:73" ht="22" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.35">
       <c r="C26">
         <v>0</v>
       </c>
@@ -13455,7 +13278,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>27</v>
       </c>
@@ -13744,7 +13567,7 @@
         <v>0.96864675610454498</v>
       </c>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>29</v>
       </c>
@@ -14033,7 +13856,7 @@
         <v>0.9960808578779623</v>
       </c>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -14322,7 +14145,7 @@
         <v>0.98604189770297412</v>
       </c>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>41</v>
       </c>
@@ -14611,7 +14434,7 @@
         <v>0.98744309417195952</v>
       </c>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -14900,7 +14723,7 @@
         <v>0.99999999901056857</v>
       </c>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -15189,7 +15012,7 @@
         <v>0.8877834661564773</v>
       </c>
     </row>
-    <row r="33" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -15478,7 +15301,7 @@
         <v>0.99260488246384015</v>
       </c>
     </row>
-    <row r="34" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -15767,7 +15590,7 @@
         <v>0.94049868236716638</v>
       </c>
     </row>
-    <row r="35" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -16056,7 +15879,7 @@
         <v>0.9964176201456928</v>
       </c>
     </row>
-    <row r="36" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -16345,7 +16168,7 @@
         <v>0.98749909623218113</v>
       </c>
     </row>
-    <row r="37" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -16634,7 +16457,7 @@
         <v>0.94809341565716188</v>
       </c>
     </row>
-    <row r="38" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -16923,7 +16746,7 @@
         <v>0.97745349576445428</v>
       </c>
     </row>
-    <row r="39" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -17212,7 +17035,7 @@
         <v>0.99861736150173053</v>
       </c>
     </row>
-    <row r="40" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -17501,7 +17324,7 @@
         <v>0.81815164815773878</v>
       </c>
     </row>
-    <row r="41" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -17790,7 +17613,7 @@
         <v>0.97665058093177115</v>
       </c>
     </row>
-    <row r="42" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
@@ -18079,42 +17902,42 @@
         <v>0.99748734272093731</v>
       </c>
     </row>
-    <row r="43" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:73" x14ac:dyDescent="0.35">
       <c r="W43" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="2:73" ht="22.5" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:73" ht="22" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:73" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:73" ht="17.5" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="21.75" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:4" ht="20.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C52" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>9</v>
       </c>
@@ -18122,7 +17945,7 @@
         <v>27.9</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>10</v>
       </c>
@@ -18130,7 +17953,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>11</v>
       </c>
@@ -18138,7 +17961,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B56">
         <v>21</v>
       </c>
@@ -18146,7 +17969,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B57">
         <v>22</v>
       </c>
@@ -18154,7 +17977,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B58">
         <v>23</v>
       </c>
@@ -18165,7 +17988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B59">
         <v>24</v>
       </c>
@@ -18173,7 +17996,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B60">
         <v>25</v>
       </c>
@@ -18181,7 +18004,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B61">
         <v>26</v>
       </c>
@@ -18189,7 +18012,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B62">
         <v>27</v>
       </c>
@@ -18197,7 +18020,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B63">
         <v>28</v>
       </c>
@@ -18205,7 +18028,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B64">
         <v>29</v>
       </c>
@@ -18213,7 +18036,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>12</v>
       </c>
@@ -18221,7 +18044,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="66" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B66">
         <v>31</v>
       </c>
@@ -18229,7 +18052,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>13</v>
       </c>
@@ -18237,7 +18060,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="68" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>23</v>
       </c>
@@ -18249,12 +18072,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:73" x14ac:dyDescent="0.35">
       <c r="C71">
         <v>0</v>
       </c>
@@ -18469,7 +18292,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>27</v>
       </c>
@@ -18758,7 +18581,7 @@
         <v>3.1353243895455019E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>29</v>
       </c>
@@ -19047,7 +18870,7 @@
         <v>3.9191421220376998E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>42</v>
       </c>
@@ -19336,7 +19159,7 @@
         <v>1.3958102297025876E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>41</v>
       </c>
@@ -19625,7 +19448,7 @@
         <v>1.2556905828040477E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>30</v>
       </c>
@@ -19914,7 +19737,7 @@
         <v>9.8943142567975428E-10</v>
       </c>
     </row>
-    <row r="77" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>31</v>
       </c>
@@ -20203,7 +20026,7 @@
         <v>0.1122165338435227</v>
       </c>
     </row>
-    <row r="78" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>32</v>
       </c>
@@ -20492,7 +20315,7 @@
         <v>7.3951175361598454E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>33</v>
       </c>
@@ -20781,7 +20604,7 @@
         <v>5.9501317632833617E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>34</v>
       </c>
@@ -21070,7 +20893,7 @@
         <v>3.582379854307205E-3</v>
       </c>
     </row>
-    <row r="81" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>35</v>
       </c>
@@ -21359,7 +21182,7 @@
         <v>1.2500903767818872E-2</v>
       </c>
     </row>
-    <row r="82" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>36</v>
       </c>
@@ -21648,7 +21471,7 @@
         <v>5.1906584342838125E-2</v>
       </c>
     </row>
-    <row r="83" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>37</v>
       </c>
@@ -21937,7 +21760,7 @@
         <v>2.2546504235545717E-2</v>
       </c>
     </row>
-    <row r="84" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>38</v>
       </c>
@@ -22226,7 +22049,7 @@
         <v>1.3826384982694728E-3</v>
       </c>
     </row>
-    <row r="85" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>39</v>
       </c>
@@ -22515,7 +22338,7 @@
         <v>0.18184835184226122</v>
       </c>
     </row>
-    <row r="86" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>40</v>
       </c>
@@ -22804,7 +22627,7 @@
         <v>2.3349419068228849E-2</v>
       </c>
     </row>
-    <row r="87" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B87" s="1" t="s">
         <v>43</v>
       </c>
@@ -23092,7 +22915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B88" s="12" t="s">
         <v>59</v>
       </c>
@@ -23381,7 +23204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:73" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:73" x14ac:dyDescent="0.35">
       <c r="B89" s="12" t="s">
         <v>60</v>
       </c>
@@ -23680,19 +23503,19 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:HC6"/>
+  <dimension ref="A1:EV6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="211" width="10.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="41.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="152" width="10.453125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:152" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -24149,647 +23972,470 @@
       <c r="EV1" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="EW1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:152" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>215</v>
-      </c>
-      <c r="EX1" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="EY1" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="EZ1" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="FA1" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="FB1" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="FC1" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="FD1" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="FE1" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="FF1" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="FG1" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="FH1" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="FI1" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="FJ1" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="FK1" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="FL1" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="FM1" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="FN1" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="FO1" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="FP1" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="FQ1" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="FR1" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="FS1" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="FT1" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="FU1" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="FV1" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="FW1" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="FX1" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="FY1" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="FZ1" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="GA1" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="GB1" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="GC1" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="GD1" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="GE1" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="GF1" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="GG1" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="GH1" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="GI1" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="GJ1" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="GK1" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="GL1" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="GM1" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="GN1" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="GO1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="GP1" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="GQ1" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="GR1" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="GS1" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="GT1" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="GU1" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="GV1" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="GW1" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="GX1" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="GY1" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="GZ1" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="HA1" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="HB1" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="HC1" s="13" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="2" spans="1:211" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>274</v>
       </c>
       <c r="B2" s="13">
         <v>0</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="13" cm="1">
+        <f t="array" ref="C2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(D2:$EV2,"&gt;0")+1)</f>
+        <v>1.2902460751168589E-4</v>
+      </c>
+      <c r="D2" s="13" cm="1">
+        <f t="array" ref="D2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(E2:$EV2,"&gt;0")+1)</f>
+        <v>1.4914252046243045E-4</v>
+      </c>
+      <c r="E2" s="13" cm="1">
+        <f t="array" ref="E2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(F2:$EV2,"&gt;0")+1)</f>
+        <v>1.7213401064802459E-4</v>
+      </c>
+      <c r="F2" s="13" cm="1">
+        <f t="array" ref="F2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(G2:$EV2,"&gt;0")+1)</f>
+        <v>1.9836517321922148E-4</v>
+      </c>
+      <c r="G2" s="13" cm="1">
+        <f t="array" ref="G2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(H2:$EV2,"&gt;0")+1)</f>
+        <v>2.2824164584198472E-4</v>
+      </c>
+      <c r="H2" s="13" cm="1">
+        <f t="array" ref="H2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(I2:$EV2,"&gt;0")+1)</f>
+        <v>2.6221179536210331E-4</v>
+      </c>
+      <c r="I2" s="13" cm="1">
+        <f t="array" ref="I2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(J2:$EV2,"&gt;0")+1)</f>
+        <v>3.0076999831803647E-4</v>
+      </c>
+      <c r="J2" s="13" cm="1">
+        <f t="array" ref="J2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(K2:$EV2,"&gt;0")+1)</f>
+        <v>3.4445999059300831E-4</v>
+      </c>
+      <c r="K2" s="13" cm="1">
+        <f t="array" ref="K2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(L2:$EV2,"&gt;0")+1)</f>
+        <v>3.9387825617268914E-4</v>
+      </c>
+      <c r="L2" s="13" cm="1">
+        <f t="array" ref="L2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(M2:$EV2,"&gt;0")+1)</f>
+        <v>4.4967741919328035E-4</v>
+      </c>
+      <c r="M2" s="13" cm="1">
+        <f t="array" ref="M2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(N2:$EV2,"&gt;0")+1)</f>
+        <v>5.1256959724925531E-4</v>
+      </c>
+      <c r="N2" s="13" cm="1">
+        <f t="array" ref="N2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(O2:$EV2,"&gt;0")+1)</f>
+        <v>5.8332966731474128E-4</v>
+      </c>
+      <c r="O2" s="13" cm="1">
+        <f t="array" ref="O2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(P2:$EV2,"&gt;0")+1)</f>
+        <v>6.6279838866684841E-4</v>
+      </c>
+      <c r="P2" s="13" cm="1">
+        <f t="array" ref="P2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(Q2:$EV2,"&gt;0")+1)</f>
+        <v>7.518853199470865E-4</v>
+      </c>
+      <c r="Q2" s="13" cm="1">
+        <f t="array" ref="Q2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(R2:$EV2,"&gt;0")+1)</f>
+        <v>8.5157146003963515E-4</v>
+      </c>
+      <c r="R2" s="13" cm="1">
+        <f t="array" ref="R2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(S2:$EV2,"&gt;0")+1)</f>
+        <v>9.6291153488170501E-4</v>
+      </c>
+      <c r="S2" s="13" cm="1">
+        <f t="array" ref="S2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(T2:$EV2,"&gt;0")+1)</f>
+        <v>1.0870358447696794E-3</v>
+      </c>
+      <c r="T2" s="13" cm="1">
+        <f t="array" ref="T2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(U2:$EV2,"&gt;0")+1)</f>
+        <v>1.2251515793226019E-3</v>
+      </c>
+      <c r="U2" s="13" cm="1">
+        <f t="array" ref="U2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(V2:$EV2,"&gt;0")+1)</f>
+        <v>1.3785435001700741E-3</v>
+      </c>
+      <c r="V2" s="13" cm="1">
+        <f t="array" ref="V2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(W2:$EV2,"&gt;0")+1)</f>
+        <v>1.5485738848218294E-3</v>
+      </c>
+      <c r="W2" s="13" cm="1">
+        <f t="array" ref="W2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(X2:$EV2,"&gt;0")+1)</f>
+        <v>1.7366816192489155E-3</v>
+      </c>
+      <c r="X2" s="13" cm="1">
+        <f t="array" ref="X2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(Y2:$EV2,"&gt;0")+1)</f>
+        <v>1.9443803216760904E-3</v>
+      </c>
+      <c r="Y2" s="13" cm="1">
+        <f t="array" ref="Y2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(Z2:$EV2,"&gt;0")+1)</f>
+        <v>2.1732553761843387E-3</v>
+      </c>
+      <c r="Z2" s="13" cm="1">
+        <f t="array" ref="Z2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AA2:$EV2,"&gt;0")+1)</f>
+        <v>2.4249597521971227E-3</v>
+      </c>
+      <c r="AA2" s="13" cm="1">
+        <f t="array" ref="AA2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AB2:$EV2,"&gt;0")+1)</f>
+        <v>2.7012084850304742E-3</v>
+      </c>
+      <c r="AB2" s="13" cm="1">
+        <f t="array" ref="AB2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AC2:$EV2,"&gt;0")+1)</f>
+        <v>3.0037716936904438E-3</v>
+      </c>
+      <c r="AC2" s="13" cm="1">
+        <f t="array" ref="AC2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AD2:$EV2,"&gt;0")+1)</f>
+        <v>3.3344660152662205E-3</v>
+      </c>
+      <c r="AD2" s="13" cm="1">
+        <f t="array" ref="AD2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AE2:$EV2,"&gt;0")+1)</f>
+        <v>3.6951443408575271E-3</v>
+      </c>
+      <c r="AE2" s="13" cm="1">
+        <f t="array" ref="AE2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AF2:$EV2,"&gt;0")+1)</f>
+        <v>4.0876837462414366E-3</v>
+      </c>
+      <c r="AF2" s="13" cm="1">
+        <f t="array" ref="AF2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AG2:$EV2,"&gt;0")+1)</f>
+        <v>4.5139715216632589E-3</v>
+      </c>
+      <c r="AG2" s="13" cm="1">
+        <f t="array" ref="AG2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AH2:$EV2,"&gt;0")+1)</f>
+        <v>4.9758892194363457E-3</v>
+      </c>
+      <c r="AH2" s="13" cm="1">
+        <f t="array" ref="AH2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AI2:$EV2,"&gt;0")+1)</f>
+        <v>5.475294655632611E-3</v>
+      </c>
+      <c r="AI2" s="13" cm="1">
+        <f t="array" ref="AI2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AJ2:$EV2,"&gt;0")+1)</f>
+        <v>6.0140018231694533E-3</v>
+      </c>
+      <c r="AJ2" s="13" cm="1">
+        <f t="array" ref="AJ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AK2:$EV2,"&gt;0")+1)</f>
+        <v>6.5937586981261028E-3</v>
+      </c>
+      <c r="AK2" s="13" cm="1">
+        <f t="array" ref="AK2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AL2:$EV2,"&gt;0")+1)</f>
+        <v>7.216222949165344E-3</v>
+      </c>
+      <c r="AL2" s="13" cm="1">
+        <f t="array" ref="AL2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AM2:$EV2,"&gt;0")+1)</f>
+        <v>7.8829355914309188E-3</v>
+      </c>
+      <c r="AM2" s="13" cm="1">
+        <f t="array" ref="AM2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AN2:$EV2,"&gt;0")+1)</f>
+        <v>8.5952926610867713E-3</v>
+      </c>
+      <c r="AN2" s="13" cm="1">
+        <f t="array" ref="AN2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AO2:$EV2,"&gt;0")+1)</f>
+        <v>9.3545150245137477E-3</v>
+      </c>
+      <c r="AO2" s="13" cm="1">
+        <f t="array" ref="AO2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AP2:$EV2,"&gt;0")+1)</f>
+        <v>1.016161647672624E-2</v>
+      </c>
+      <c r="AP2" s="13" cm="1">
+        <f t="array" ref="AP2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AQ2:$EV2,"&gt;0")+1)</f>
+        <v>1.1017370326340984E-2</v>
+      </c>
+      <c r="AQ2" s="13" cm="1">
+        <f t="array" ref="AQ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AR2:$EV2,"&gt;0")+1)</f>
+        <v>1.1922274708817428E-2</v>
+      </c>
+      <c r="AR2" s="13" cm="1">
+        <f t="array" ref="AR2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AS2:$EV2,"&gt;0")+1)</f>
+        <v>1.2876516914949086E-2</v>
+      </c>
+      <c r="AS2" s="13" cm="1">
+        <f t="array" ref="AS2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AT2:$EV2,"&gt;0")+1)</f>
+        <v>1.3879937066821351E-2</v>
+      </c>
+      <c r="AT2" s="13" cm="1">
+        <f t="array" ref="AT2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AU2:$EV2,"&gt;0")+1)</f>
+        <v>1.493199151760132E-2</v>
+      </c>
+      <c r="AU2" s="13" cm="1">
+        <f t="array" ref="AU2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AV2:$EV2,"&gt;0")+1)</f>
+        <v>1.6031716393348442E-2</v>
+      </c>
+      <c r="AV2" s="13" cm="1">
+        <f t="array" ref="AV2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AW2:$EV2,"&gt;0")+1)</f>
+        <v>1.7177691733087225E-2</v>
+      </c>
+      <c r="AW2" s="13" cm="1">
+        <f t="array" ref="AW2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AX2:$EV2,"&gt;0")+1)</f>
+        <v>1.8368006715991817E-2</v>
+      </c>
+      <c r="AX2" s="13" cm="1">
+        <f t="array" ref="AX2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AY2:$EV2,"&gt;0")+1)</f>
+        <v>1.9600226489744185E-2</v>
+      </c>
+      <c r="AY2" s="13" cm="1">
+        <f t="array" ref="AY2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(AZ2:$EV2,"&gt;0")+1)</f>
+        <v>2.0871361129648641E-2</v>
+      </c>
+      <c r="AZ2" s="13" cm="1">
+        <f t="array" ref="AZ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BA2:$EV2,"&gt;0")+1)</f>
+        <v>2.2177837261161858E-2</v>
+      </c>
+      <c r="BA2" s="13" cm="1">
+        <f t="array" ref="BA2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BB2:$EV2,"&gt;0")+1)</f>
+        <v>2.351547286575012E-2</v>
+      </c>
+      <c r="BB2" s="13" cm="1">
+        <f t="array" ref="BB2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BC2:$EV2,"&gt;0")+1)</f>
+        <v>2.4879455757128115E-2</v>
+      </c>
+      <c r="BC2" s="13" cm="1">
+        <f t="array" ref="BC2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BD2:$EV2,"&gt;0")+1)</f>
+        <v>2.6264326156322966E-2</v>
+      </c>
+      <c r="BD2" s="13" cm="1">
+        <f t="array" ref="BD2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BE2:$EV2,"&gt;0")+1)</f>
+        <v>2.7663963701903473E-2</v>
+      </c>
+      <c r="BE2" s="13" cm="1">
+        <f t="array" ref="BE2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BF2:$EV2,"&gt;0")+1)</f>
+        <v>2.9071579095045944E-2</v>
+      </c>
+      <c r="BF2" s="13" cm="1">
+        <f t="array" ref="BF2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BG2:$EV2,"&gt;0")+1)</f>
+        <v>3.047971038136614E-2</v>
+      </c>
+      <c r="BG2" s="13" cm="1">
+        <f t="array" ref="BG2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BH2:$EV2,"&gt;0")+1)</f>
+        <v>3.1880223587013021E-2</v>
+      </c>
+      <c r="BH2" s="13" cm="1">
+        <f t="array" ref="BH2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BI2:$EV2,"&gt;0")+1)</f>
+        <v>3.3264317014074632E-2</v>
+      </c>
+      <c r="BI2" s="13" cm="1">
+        <f t="array" ref="BI2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BJ2:$EV2,"&gt;0")+1)</f>
+        <v>3.4622527890620806E-2</v>
+      </c>
+      <c r="BJ2" s="13" cm="1">
+        <f t="array" ref="BJ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BK2:$EV2,"&gt;0")+1)</f>
+        <v>3.5944739142854523E-2</v>
+      </c>
+      <c r="BK2" s="13" cm="1">
+        <f t="array" ref="BK2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BL2:$EV2,"&gt;0")+1)</f>
+        <v>3.7220182590675631E-2</v>
+      </c>
+      <c r="BL2" s="13" cm="1">
+        <f t="array" ref="BL2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BM2:$EV2,"&gt;0")+1)</f>
+        <v>3.8437432442177975E-2</v>
+      </c>
+      <c r="BM2" s="13" cm="1">
+        <f t="array" ref="BM2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BN2:$EV2,"&gt;0")+1)</f>
+        <v>3.9584378723700436E-2</v>
+      </c>
+      <c r="BN2" s="13" cm="1">
+        <f t="array" ref="BN2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BO2:$EV2,"&gt;0")+1)</f>
+        <v>4.0648162378080624E-2</v>
+      </c>
+      <c r="BO2" s="13" cm="1">
+        <f t="array" ref="BO2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BP2:$EV2,"&gt;0")+1)</f>
+        <v>4.1615037820234152E-2</v>
+      </c>
+      <c r="BP2" s="13" cm="1">
+        <f t="array" ref="BP2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BQ2:$EV2,"&gt;0")+1)</f>
+        <v>4.2470093237806192E-2</v>
+      </c>
+      <c r="BQ2" s="13" cm="1">
+        <f t="array" ref="BQ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BR2:$EV2,"&gt;0")+1)</f>
+        <v>4.3196668790199171E-2</v>
+      </c>
+      <c r="BR2" s="13" cm="1">
+        <f t="array" ref="BR2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BS2:$EV2,"&gt;0")+1)</f>
+        <v>4.3775036452648193E-2</v>
+      </c>
+      <c r="BS2" s="13" cm="1">
+        <f t="array" ref="BS2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BT2:$EV2,"&gt;0")+1)</f>
+        <v>4.4178746006988449E-2</v>
+      </c>
+      <c r="BT2" s="13" cm="1">
+        <f t="array" ref="BT2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BU2:$EV2,"&gt;0")+1)</f>
+        <v>4.4355689542047459E-2</v>
+      </c>
+      <c r="BU2" s="13">
         <v>0</v>
       </c>
-      <c r="D2" s="13">
+      <c r="BV2" s="13">
         <v>0</v>
       </c>
-      <c r="E2" s="13">
+      <c r="BW2" s="13">
         <v>0</v>
       </c>
-      <c r="F2" s="13">
+      <c r="BX2" s="13">
         <v>0</v>
       </c>
-      <c r="G2" s="13">
+      <c r="BY2" s="13">
         <v>0</v>
       </c>
-      <c r="H2" s="13">
+      <c r="BZ2" s="13">
         <v>0</v>
       </c>
-      <c r="I2" s="13">
+      <c r="CA2" s="13">
         <v>0</v>
       </c>
-      <c r="J2" s="13">
+      <c r="CB2" s="13">
         <v>0</v>
       </c>
-      <c r="K2" s="13">
+      <c r="CC2" s="13">
         <v>0</v>
       </c>
-      <c r="L2" s="13">
+      <c r="CD2" s="13">
         <v>0</v>
       </c>
-      <c r="M2" s="13">
+      <c r="CE2" s="13">
         <v>0</v>
       </c>
-      <c r="N2" s="13">
+      <c r="CF2" s="13">
         <v>0</v>
       </c>
-      <c r="O2" s="13">
+      <c r="CG2" s="13">
         <v>0</v>
       </c>
-      <c r="P2" s="13">
+      <c r="CH2" s="13">
         <v>0</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="CI2" s="13">
         <v>0</v>
       </c>
-      <c r="R2" s="13">
+      <c r="CJ2" s="13">
         <v>0</v>
       </c>
-      <c r="S2" s="13">
+      <c r="CK2" s="13">
         <v>0</v>
       </c>
-      <c r="T2" s="13">
+      <c r="CL2" s="13">
         <v>0</v>
       </c>
-      <c r="U2" s="13">
+      <c r="CM2" s="13">
         <v>0</v>
       </c>
-      <c r="V2" s="13">
+      <c r="CN2" s="13">
         <v>0</v>
       </c>
-      <c r="W2" s="13">
+      <c r="CO2" s="13">
         <v>0</v>
       </c>
-      <c r="X2" s="13">
+      <c r="CP2" s="13">
         <v>0</v>
       </c>
-      <c r="Y2" s="13">
+      <c r="CQ2" s="13">
         <v>0</v>
       </c>
-      <c r="Z2" s="13">
+      <c r="CR2" s="13">
         <v>0</v>
       </c>
-      <c r="AA2" s="13">
+      <c r="CS2" s="13">
         <v>0</v>
       </c>
-      <c r="AB2" s="13">
+      <c r="CT2" s="13">
         <v>0</v>
       </c>
-      <c r="AC2" s="13">
+      <c r="CU2" s="13">
         <v>0</v>
       </c>
-      <c r="AD2" s="13">
+      <c r="CV2" s="13">
         <v>0</v>
       </c>
-      <c r="AE2" s="13">
+      <c r="CW2" s="13">
         <v>0</v>
       </c>
-      <c r="AF2" s="13">
+      <c r="CX2" s="13">
         <v>0</v>
       </c>
-      <c r="AG2" s="13">
+      <c r="CY2" s="13">
         <v>0</v>
       </c>
-      <c r="AH2" s="13">
+      <c r="CZ2" s="13">
         <v>0</v>
       </c>
-      <c r="AI2" s="13">
+      <c r="DA2" s="13">
         <v>0</v>
       </c>
-      <c r="AJ2" s="13">
+      <c r="DB2" s="13">
         <v>0</v>
       </c>
-      <c r="AK2" s="13">
+      <c r="DC2" s="13">
         <v>0</v>
       </c>
-      <c r="AL2" s="13">
+      <c r="DD2" s="13">
         <v>0</v>
       </c>
-      <c r="AM2" s="13">
+      <c r="DE2" s="13">
         <v>0</v>
       </c>
-      <c r="AN2" s="13">
+      <c r="DF2" s="13">
         <v>0</v>
       </c>
-      <c r="AO2" s="13">
+      <c r="DG2" s="13">
         <v>0</v>
       </c>
-      <c r="AP2" s="13">
+      <c r="DH2" s="13">
         <v>0</v>
       </c>
-      <c r="AQ2" s="13">
+      <c r="DI2" s="13">
         <v>0</v>
       </c>
-      <c r="AR2" s="13">
+      <c r="DJ2" s="13">
         <v>0</v>
       </c>
-      <c r="AS2" s="13">
+      <c r="DK2" s="13">
         <v>0</v>
       </c>
-      <c r="AT2" s="13">
+      <c r="DL2" s="13">
         <v>0</v>
       </c>
-      <c r="AU2" s="13">
+      <c r="DM2" s="13">
         <v>0</v>
       </c>
-      <c r="AV2" s="13">
+      <c r="DN2" s="13">
         <v>0</v>
       </c>
-      <c r="AW2" s="13">
+      <c r="DO2" s="13">
         <v>0</v>
       </c>
-      <c r="AX2" s="13">
+      <c r="DP2" s="13">
         <v>0</v>
       </c>
-      <c r="AY2" s="13">
+      <c r="DQ2" s="13">
         <v>0</v>
       </c>
-      <c r="AZ2" s="13">
+      <c r="DR2" s="13">
         <v>0</v>
       </c>
-      <c r="BA2" s="13">
+      <c r="DS2" s="13">
         <v>0</v>
       </c>
-      <c r="BB2" s="13">
+      <c r="DT2" s="13">
         <v>0</v>
       </c>
-      <c r="BC2" s="13">
+      <c r="DU2" s="13">
         <v>0</v>
       </c>
-      <c r="BD2" s="13">
+      <c r="DV2" s="13">
         <v>0</v>
       </c>
-      <c r="BE2" s="13">
+      <c r="DW2" s="13">
         <v>0</v>
       </c>
-      <c r="BF2" s="13">
+      <c r="DX2" s="13">
         <v>0</v>
       </c>
-      <c r="BG2" s="13">
+      <c r="DY2" s="13">
         <v>0</v>
       </c>
-      <c r="BH2" s="13">
+      <c r="DZ2" s="13">
         <v>0</v>
       </c>
-      <c r="BI2" s="13">
+      <c r="EA2" s="13">
         <v>0</v>
-      </c>
-      <c r="BJ2" s="13" cm="1">
-        <f t="array" ref="BJ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BK2:$HC2,"&gt;0")+1)</f>
-        <v>1.2902460751168589E-4</v>
-      </c>
-      <c r="BK2" s="13" cm="1">
-        <f t="array" ref="BK2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BL2:$HC2,"&gt;0")+1)</f>
-        <v>1.4914252046243045E-4</v>
-      </c>
-      <c r="BL2" s="13" cm="1">
-        <f t="array" ref="BL2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BM2:$HC2,"&gt;0")+1)</f>
-        <v>1.7213401064802459E-4</v>
-      </c>
-      <c r="BM2" s="13" cm="1">
-        <f t="array" ref="BM2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BN2:$HC2,"&gt;0")+1)</f>
-        <v>1.9836517321922148E-4</v>
-      </c>
-      <c r="BN2" s="13" cm="1">
-        <f t="array" ref="BN2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BO2:$HC2,"&gt;0")+1)</f>
-        <v>2.2824164584198472E-4</v>
-      </c>
-      <c r="BO2" s="13" cm="1">
-        <f t="array" ref="BO2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BP2:$HC2,"&gt;0")+1)</f>
-        <v>2.6221179536210331E-4</v>
-      </c>
-      <c r="BP2" s="13" cm="1">
-        <f t="array" ref="BP2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BQ2:$HC2,"&gt;0")+1)</f>
-        <v>3.0076999831803647E-4</v>
-      </c>
-      <c r="BQ2" s="13" cm="1">
-        <f t="array" ref="BQ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BR2:$HC2,"&gt;0")+1)</f>
-        <v>3.4445999059300831E-4</v>
-      </c>
-      <c r="BR2" s="13" cm="1">
-        <f t="array" ref="BR2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BS2:$HC2,"&gt;0")+1)</f>
-        <v>3.9387825617268914E-4</v>
-      </c>
-      <c r="BS2" s="13" cm="1">
-        <f t="array" ref="BS2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BT2:$HC2,"&gt;0")+1)</f>
-        <v>4.4967741919328035E-4</v>
-      </c>
-      <c r="BT2" s="13" cm="1">
-        <f t="array" ref="BT2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BU2:$HC2,"&gt;0")+1)</f>
-        <v>5.1256959724925531E-4</v>
-      </c>
-      <c r="BU2" s="13" cm="1">
-        <f t="array" ref="BU2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BV2:$HC2,"&gt;0")+1)</f>
-        <v>5.8332966731474128E-4</v>
-      </c>
-      <c r="BV2" s="13" cm="1">
-        <f t="array" ref="BV2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BW2:$HC2,"&gt;0")+1)</f>
-        <v>6.6279838866684841E-4</v>
-      </c>
-      <c r="BW2" s="13" cm="1">
-        <f t="array" ref="BW2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BX2:$HC2,"&gt;0")+1)</f>
-        <v>7.518853199470865E-4</v>
-      </c>
-      <c r="BX2" s="13" cm="1">
-        <f t="array" ref="BX2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BY2:$HC2,"&gt;0")+1)</f>
-        <v>8.5157146003963515E-4</v>
-      </c>
-      <c r="BY2" s="13" cm="1">
-        <f t="array" ref="BY2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(BZ2:$HC2,"&gt;0")+1)</f>
-        <v>9.6291153488170501E-4</v>
-      </c>
-      <c r="BZ2" s="13" cm="1">
-        <f t="array" ref="BZ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CA2:$HC2,"&gt;0")+1)</f>
-        <v>1.0870358447696794E-3</v>
-      </c>
-      <c r="CA2" s="13" cm="1">
-        <f t="array" ref="CA2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CB2:$HC2,"&gt;0")+1)</f>
-        <v>1.2251515793226019E-3</v>
-      </c>
-      <c r="CB2" s="13" cm="1">
-        <f t="array" ref="CB2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CC2:$HC2,"&gt;0")+1)</f>
-        <v>1.3785435001700741E-3</v>
-      </c>
-      <c r="CC2" s="13" cm="1">
-        <f t="array" ref="CC2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CD2:$HC2,"&gt;0")+1)</f>
-        <v>1.5485738848218294E-3</v>
-      </c>
-      <c r="CD2" s="13" cm="1">
-        <f t="array" ref="CD2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CE2:$HC2,"&gt;0")+1)</f>
-        <v>1.7366816192489155E-3</v>
-      </c>
-      <c r="CE2" s="13" cm="1">
-        <f t="array" ref="CE2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CF2:$HC2,"&gt;0")+1)</f>
-        <v>1.9443803216760904E-3</v>
-      </c>
-      <c r="CF2" s="13" cm="1">
-        <f t="array" ref="CF2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CG2:$HC2,"&gt;0")+1)</f>
-        <v>2.1732553761843387E-3</v>
-      </c>
-      <c r="CG2" s="13" cm="1">
-        <f t="array" ref="CG2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CH2:$HC2,"&gt;0")+1)</f>
-        <v>2.4249597521971227E-3</v>
-      </c>
-      <c r="CH2" s="13" cm="1">
-        <f t="array" ref="CH2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CI2:$HC2,"&gt;0")+1)</f>
-        <v>2.7012084850304742E-3</v>
-      </c>
-      <c r="CI2" s="13" cm="1">
-        <f t="array" ref="CI2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CJ2:$HC2,"&gt;0")+1)</f>
-        <v>3.0037716936904438E-3</v>
-      </c>
-      <c r="CJ2" s="13" cm="1">
-        <f t="array" ref="CJ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CK2:$HC2,"&gt;0")+1)</f>
-        <v>3.3344660152662205E-3</v>
-      </c>
-      <c r="CK2" s="13" cm="1">
-        <f t="array" ref="CK2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CL2:$HC2,"&gt;0")+1)</f>
-        <v>3.6951443408575271E-3</v>
-      </c>
-      <c r="CL2" s="13" cm="1">
-        <f t="array" ref="CL2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CM2:$HC2,"&gt;0")+1)</f>
-        <v>4.0876837462414366E-3</v>
-      </c>
-      <c r="CM2" s="13" cm="1">
-        <f t="array" ref="CM2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CN2:$HC2,"&gt;0")+1)</f>
-        <v>4.5139715216632589E-3</v>
-      </c>
-      <c r="CN2" s="13" cm="1">
-        <f t="array" ref="CN2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CO2:$HC2,"&gt;0")+1)</f>
-        <v>4.9758892194363457E-3</v>
-      </c>
-      <c r="CO2" s="13" cm="1">
-        <f t="array" ref="CO2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CP2:$HC2,"&gt;0")+1)</f>
-        <v>5.475294655632611E-3</v>
-      </c>
-      <c r="CP2" s="13" cm="1">
-        <f t="array" ref="CP2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CQ2:$HC2,"&gt;0")+1)</f>
-        <v>6.0140018231694533E-3</v>
-      </c>
-      <c r="CQ2" s="13" cm="1">
-        <f t="array" ref="CQ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CR2:$HC2,"&gt;0")+1)</f>
-        <v>6.5937586981261028E-3</v>
-      </c>
-      <c r="CR2" s="13" cm="1">
-        <f t="array" ref="CR2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CS2:$HC2,"&gt;0")+1)</f>
-        <v>7.216222949165344E-3</v>
-      </c>
-      <c r="CS2" s="13" cm="1">
-        <f t="array" ref="CS2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CT2:$HC2,"&gt;0")+1)</f>
-        <v>7.8829355914309188E-3</v>
-      </c>
-      <c r="CT2" s="13" cm="1">
-        <f t="array" ref="CT2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CU2:$HC2,"&gt;0")+1)</f>
-        <v>8.5952926610867713E-3</v>
-      </c>
-      <c r="CU2" s="13" cm="1">
-        <f t="array" ref="CU2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CV2:$HC2,"&gt;0")+1)</f>
-        <v>9.3545150245137477E-3</v>
-      </c>
-      <c r="CV2" s="13" cm="1">
-        <f t="array" ref="CV2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CW2:$HC2,"&gt;0")+1)</f>
-        <v>1.016161647672624E-2</v>
-      </c>
-      <c r="CW2" s="13" cm="1">
-        <f t="array" ref="CW2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CX2:$HC2,"&gt;0")+1)</f>
-        <v>1.1017370326340984E-2</v>
-      </c>
-      <c r="CX2" s="13" cm="1">
-        <f t="array" ref="CX2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CY2:$HC2,"&gt;0")+1)</f>
-        <v>1.1922274708817428E-2</v>
-      </c>
-      <c r="CY2" s="13" cm="1">
-        <f t="array" ref="CY2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(CZ2:$HC2,"&gt;0")+1)</f>
-        <v>1.2876516914949086E-2</v>
-      </c>
-      <c r="CZ2" s="13" cm="1">
-        <f t="array" ref="CZ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DA2:$HC2,"&gt;0")+1)</f>
-        <v>1.3879937066821351E-2</v>
-      </c>
-      <c r="DA2" s="13" cm="1">
-        <f t="array" ref="DA2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DB2:$HC2,"&gt;0")+1)</f>
-        <v>1.493199151760132E-2</v>
-      </c>
-      <c r="DB2" s="13" cm="1">
-        <f t="array" ref="DB2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DC2:$HC2,"&gt;0")+1)</f>
-        <v>1.6031716393348442E-2</v>
-      </c>
-      <c r="DC2" s="13" cm="1">
-        <f t="array" ref="DC2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DD2:$HC2,"&gt;0")+1)</f>
-        <v>1.7177691733087225E-2</v>
-      </c>
-      <c r="DD2" s="13" cm="1">
-        <f t="array" ref="DD2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DE2:$HC2,"&gt;0")+1)</f>
-        <v>1.8368006715991817E-2</v>
-      </c>
-      <c r="DE2" s="13" cm="1">
-        <f t="array" ref="DE2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DF2:$HC2,"&gt;0")+1)</f>
-        <v>1.9600226489744185E-2</v>
-      </c>
-      <c r="DF2" s="13" cm="1">
-        <f t="array" ref="DF2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DG2:$HC2,"&gt;0")+1)</f>
-        <v>2.0871361129648641E-2</v>
-      </c>
-      <c r="DG2" s="13" cm="1">
-        <f t="array" ref="DG2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DH2:$HC2,"&gt;0")+1)</f>
-        <v>2.2177837261161858E-2</v>
-      </c>
-      <c r="DH2" s="13" cm="1">
-        <f t="array" ref="DH2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DI2:$HC2,"&gt;0")+1)</f>
-        <v>2.351547286575012E-2</v>
-      </c>
-      <c r="DI2" s="13" cm="1">
-        <f t="array" ref="DI2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DJ2:$HC2,"&gt;0")+1)</f>
-        <v>2.4879455757128115E-2</v>
-      </c>
-      <c r="DJ2" s="13" cm="1">
-        <f t="array" ref="DJ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DK2:$HC2,"&gt;0")+1)</f>
-        <v>2.6264326156322966E-2</v>
-      </c>
-      <c r="DK2" s="13" cm="1">
-        <f t="array" ref="DK2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DL2:$HC2,"&gt;0")+1)</f>
-        <v>2.7663963701903473E-2</v>
-      </c>
-      <c r="DL2" s="13" cm="1">
-        <f t="array" ref="DL2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DM2:$HC2,"&gt;0")+1)</f>
-        <v>2.9071579095045944E-2</v>
-      </c>
-      <c r="DM2" s="13" cm="1">
-        <f t="array" ref="DM2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DN2:$HC2,"&gt;0")+1)</f>
-        <v>3.047971038136614E-2</v>
-      </c>
-      <c r="DN2" s="13" cm="1">
-        <f t="array" ref="DN2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DO2:$HC2,"&gt;0")+1)</f>
-        <v>3.1880223587013021E-2</v>
-      </c>
-      <c r="DO2" s="13" cm="1">
-        <f t="array" ref="DO2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DP2:$HC2,"&gt;0")+1)</f>
-        <v>3.3264317014074632E-2</v>
-      </c>
-      <c r="DP2" s="13" cm="1">
-        <f t="array" ref="DP2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DQ2:$HC2,"&gt;0")+1)</f>
-        <v>3.4622527890620806E-2</v>
-      </c>
-      <c r="DQ2" s="13" cm="1">
-        <f t="array" ref="DQ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DR2:$HC2,"&gt;0")+1)</f>
-        <v>3.5944739142854523E-2</v>
-      </c>
-      <c r="DR2" s="13" cm="1">
-        <f t="array" ref="DR2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DS2:$HC2,"&gt;0")+1)</f>
-        <v>3.7220182590675631E-2</v>
-      </c>
-      <c r="DS2" s="13" cm="1">
-        <f t="array" ref="DS2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DT2:$HC2,"&gt;0")+1)</f>
-        <v>3.8437432442177975E-2</v>
-      </c>
-      <c r="DT2" s="13" cm="1">
-        <f t="array" ref="DT2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DU2:$HC2,"&gt;0")+1)</f>
-        <v>3.9584378723700436E-2</v>
-      </c>
-      <c r="DU2" s="13" cm="1">
-        <f t="array" ref="DU2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DV2:$HC2,"&gt;0")+1)</f>
-        <v>4.0648162378080624E-2</v>
-      </c>
-      <c r="DV2" s="13" cm="1">
-        <f t="array" ref="DV2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DW2:$HC2,"&gt;0")+1)</f>
-        <v>4.1615037820234152E-2</v>
-      </c>
-      <c r="DW2" s="13" cm="1">
-        <f t="array" ref="DW2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DX2:$HC2,"&gt;0")+1)</f>
-        <v>4.2470093237806192E-2</v>
-      </c>
-      <c r="DX2" s="13" cm="1">
-        <f t="array" ref="DX2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DY2:$HC2,"&gt;0")+1)</f>
-        <v>4.3196668790199171E-2</v>
-      </c>
-      <c r="DY2" s="13" cm="1">
-        <f t="array" ref="DY2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(DZ2:$HC2,"&gt;0")+1)</f>
-        <v>4.3775036452648193E-2</v>
-      </c>
-      <c r="DZ2" s="13" cm="1">
-        <f t="array" ref="DZ2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(EA2:$HC2,"&gt;0")+1)</f>
-        <v>4.4178746006988449E-2</v>
-      </c>
-      <c r="EA2" s="13" cm="1">
-        <f t="array" ref="EA2">INDEX(Calcs!$C$88:$BU$88,COUNTIF(EB2:$HC2,"&gt;0")+1)</f>
-        <v>4.4355689542047459E-2</v>
       </c>
       <c r="EB2" s="13">
         <v>0</v>
@@ -24854,186 +24500,9 @@
       <c r="EV2" s="13">
         <v>0</v>
       </c>
-      <c r="EW2" s="13">
-        <v>0</v>
-      </c>
-      <c r="EX2" s="13">
-        <v>0</v>
-      </c>
-      <c r="EY2" s="13">
-        <v>0</v>
-      </c>
-      <c r="EZ2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FA2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FB2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FC2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FD2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FE2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FF2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FG2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FH2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FI2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FJ2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FK2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FL2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FM2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FN2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FO2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FP2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FQ2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FR2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FS2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FT2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FU2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FV2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FW2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FX2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FY2" s="13">
-        <v>0</v>
-      </c>
-      <c r="FZ2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GA2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GB2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GC2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GD2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GE2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GF2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GG2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GH2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GI2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GJ2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GK2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GL2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GM2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GN2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GO2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GP2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GQ2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GR2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GS2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GT2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GU2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GV2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GW2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GX2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GY2" s="13">
-        <v>0</v>
-      </c>
-      <c r="GZ2" s="13">
-        <v>0</v>
-      </c>
-      <c r="HA2" s="13">
-        <v>0</v>
-      </c>
-      <c r="HB2" s="13">
-        <v>0</v>
-      </c>
-      <c r="HC2" s="13">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:211" x14ac:dyDescent="0.25">
-      <c r="DV6"/>
+    <row r="6" spans="1:152" x14ac:dyDescent="0.35">
+      <c r="BO6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25045,18 +24514,18 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:HD2"/>
+  <dimension ref="A1:EW2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BS17" sqref="BS17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:212" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:153" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>0</v>
       </c>
@@ -25513,185 +24982,8 @@
       <c r="EW1">
         <v>151</v>
       </c>
-      <c r="EX1">
-        <v>152</v>
-      </c>
-      <c r="EY1">
-        <v>153</v>
-      </c>
-      <c r="EZ1">
-        <v>154</v>
-      </c>
-      <c r="FA1">
-        <v>155</v>
-      </c>
-      <c r="FB1">
-        <v>156</v>
-      </c>
-      <c r="FC1">
-        <v>157</v>
-      </c>
-      <c r="FD1">
-        <v>158</v>
-      </c>
-      <c r="FE1">
-        <v>159</v>
-      </c>
-      <c r="FF1">
-        <v>160</v>
-      </c>
-      <c r="FG1">
-        <v>161</v>
-      </c>
-      <c r="FH1">
-        <v>162</v>
-      </c>
-      <c r="FI1">
-        <v>163</v>
-      </c>
-      <c r="FJ1">
-        <v>164</v>
-      </c>
-      <c r="FK1">
-        <v>165</v>
-      </c>
-      <c r="FL1">
-        <v>166</v>
-      </c>
-      <c r="FM1">
-        <v>167</v>
-      </c>
-      <c r="FN1">
-        <v>168</v>
-      </c>
-      <c r="FO1">
-        <v>169</v>
-      </c>
-      <c r="FP1">
-        <v>170</v>
-      </c>
-      <c r="FQ1">
-        <v>171</v>
-      </c>
-      <c r="FR1">
-        <v>172</v>
-      </c>
-      <c r="FS1">
-        <v>173</v>
-      </c>
-      <c r="FT1">
-        <v>174</v>
-      </c>
-      <c r="FU1">
-        <v>175</v>
-      </c>
-      <c r="FV1">
-        <v>176</v>
-      </c>
-      <c r="FW1">
-        <v>177</v>
-      </c>
-      <c r="FX1">
-        <v>178</v>
-      </c>
-      <c r="FY1">
-        <v>179</v>
-      </c>
-      <c r="FZ1">
-        <v>180</v>
-      </c>
-      <c r="GA1">
-        <v>181</v>
-      </c>
-      <c r="GB1">
-        <v>182</v>
-      </c>
-      <c r="GC1">
-        <v>183</v>
-      </c>
-      <c r="GD1">
-        <v>184</v>
-      </c>
-      <c r="GE1">
-        <v>185</v>
-      </c>
-      <c r="GF1">
-        <v>186</v>
-      </c>
-      <c r="GG1">
-        <v>187</v>
-      </c>
-      <c r="GH1">
-        <v>188</v>
-      </c>
-      <c r="GI1">
-        <v>189</v>
-      </c>
-      <c r="GJ1">
-        <v>190</v>
-      </c>
-      <c r="GK1">
-        <v>191</v>
-      </c>
-      <c r="GL1">
-        <v>192</v>
-      </c>
-      <c r="GM1">
-        <v>193</v>
-      </c>
-      <c r="GN1">
-        <v>194</v>
-      </c>
-      <c r="GO1">
-        <v>195</v>
-      </c>
-      <c r="GP1">
-        <v>196</v>
-      </c>
-      <c r="GQ1">
-        <v>197</v>
-      </c>
-      <c r="GR1">
-        <v>198</v>
-      </c>
-      <c r="GS1">
-        <v>199</v>
-      </c>
-      <c r="GT1">
-        <v>200</v>
-      </c>
-      <c r="GU1">
-        <v>201</v>
-      </c>
-      <c r="GV1">
-        <v>202</v>
-      </c>
-      <c r="GW1">
-        <v>203</v>
-      </c>
-      <c r="GX1">
-        <v>204</v>
-      </c>
-      <c r="GY1">
-        <v>205</v>
-      </c>
-      <c r="GZ1">
-        <v>206</v>
-      </c>
-      <c r="HA1">
-        <v>207</v>
-      </c>
-      <c r="HB1">
-        <v>208</v>
-      </c>
-      <c r="HC1">
-        <v>209</v>
-      </c>
-      <c r="HD1">
-        <v>210</v>
-      </c>
     </row>
-    <row r="2" spans="1:212" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:153" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -26220,183 +25512,6 @@
         <v>1</v>
       </c>
       <c r="EW2">
-        <v>1</v>
-      </c>
-      <c r="EX2">
-        <v>1</v>
-      </c>
-      <c r="EY2">
-        <v>1</v>
-      </c>
-      <c r="EZ2">
-        <v>1</v>
-      </c>
-      <c r="FA2">
-        <v>1</v>
-      </c>
-      <c r="FB2">
-        <v>1</v>
-      </c>
-      <c r="FC2">
-        <v>1</v>
-      </c>
-      <c r="FD2">
-        <v>1</v>
-      </c>
-      <c r="FE2">
-        <v>1</v>
-      </c>
-      <c r="FF2">
-        <v>1</v>
-      </c>
-      <c r="FG2">
-        <v>1</v>
-      </c>
-      <c r="FH2">
-        <v>1</v>
-      </c>
-      <c r="FI2">
-        <v>1</v>
-      </c>
-      <c r="FJ2">
-        <v>1</v>
-      </c>
-      <c r="FK2">
-        <v>1</v>
-      </c>
-      <c r="FL2">
-        <v>1</v>
-      </c>
-      <c r="FM2">
-        <v>1</v>
-      </c>
-      <c r="FN2">
-        <v>1</v>
-      </c>
-      <c r="FO2">
-        <v>1</v>
-      </c>
-      <c r="FP2">
-        <v>1</v>
-      </c>
-      <c r="FQ2">
-        <v>1</v>
-      </c>
-      <c r="FR2">
-        <v>1</v>
-      </c>
-      <c r="FS2">
-        <v>1</v>
-      </c>
-      <c r="FT2">
-        <v>1</v>
-      </c>
-      <c r="FU2">
-        <v>1</v>
-      </c>
-      <c r="FV2">
-        <v>1</v>
-      </c>
-      <c r="FW2">
-        <v>1</v>
-      </c>
-      <c r="FX2">
-        <v>1</v>
-      </c>
-      <c r="FY2">
-        <v>1</v>
-      </c>
-      <c r="FZ2">
-        <v>1</v>
-      </c>
-      <c r="GA2">
-        <v>1</v>
-      </c>
-      <c r="GB2">
-        <v>1</v>
-      </c>
-      <c r="GC2">
-        <v>1</v>
-      </c>
-      <c r="GD2">
-        <v>1</v>
-      </c>
-      <c r="GE2">
-        <v>1</v>
-      </c>
-      <c r="GF2">
-        <v>1</v>
-      </c>
-      <c r="GG2">
-        <v>1</v>
-      </c>
-      <c r="GH2">
-        <v>1</v>
-      </c>
-      <c r="GI2">
-        <v>1</v>
-      </c>
-      <c r="GJ2">
-        <v>1</v>
-      </c>
-      <c r="GK2">
-        <v>1</v>
-      </c>
-      <c r="GL2">
-        <v>1</v>
-      </c>
-      <c r="GM2">
-        <v>1</v>
-      </c>
-      <c r="GN2">
-        <v>1</v>
-      </c>
-      <c r="GO2">
-        <v>1</v>
-      </c>
-      <c r="GP2">
-        <v>1</v>
-      </c>
-      <c r="GQ2">
-        <v>1</v>
-      </c>
-      <c r="GR2">
-        <v>1</v>
-      </c>
-      <c r="GS2">
-        <v>1</v>
-      </c>
-      <c r="GT2">
-        <v>1</v>
-      </c>
-      <c r="GU2">
-        <v>1</v>
-      </c>
-      <c r="GV2">
-        <v>1</v>
-      </c>
-      <c r="GW2">
-        <v>1</v>
-      </c>
-      <c r="GX2">
-        <v>1</v>
-      </c>
-      <c r="GY2">
-        <v>1</v>
-      </c>
-      <c r="GZ2">
-        <v>1</v>
-      </c>
-      <c r="HA2">
-        <v>1</v>
-      </c>
-      <c r="HB2">
-        <v>1</v>
-      </c>
-      <c r="HC2">
-        <v>1</v>
-      </c>
-      <c r="HD2">
         <v>1</v>
       </c>
     </row>

</xml_diff>